<commit_message>
fixed sched and added judge maker
</commit_message>
<xml_diff>
--- a/SRC/FLL Schedule.xlsx
+++ b/SRC/FLL Schedule.xlsx
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="181">
   <si>
     <t xml:space="preserve">47 Teams</t>
   </si>
@@ -189,7 +189,7 @@
     <t xml:space="preserve">Corpus Christy</t>
   </si>
   <si>
-    <t xml:space="preserve">Robot Judge: Grp1</t>
+    <t xml:space="preserve">Robot Judge Grp 1</t>
   </si>
   <si>
     <t xml:space="preserve">Field 1 Green</t>
@@ -198,7 +198,7 @@
     <t xml:space="preserve">Judge’s Break</t>
   </si>
   <si>
-    <t xml:space="preserve">Project Judge Group 1</t>
+    <t xml:space="preserve">Project Judge Grp 1</t>
   </si>
   <si>
     <t xml:space="preserve">Field: 1 Green</t>
@@ -210,15 +210,9 @@
     <t xml:space="preserve">RoboLegoLancers</t>
   </si>
   <si>
-    <t xml:space="preserve">Robot Judge: Grp 1</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t xml:space="preserve">Project Judge Grp 1</t>
-  </si>
-  <si>
     <t xml:space="preserve">Field:1 Green</t>
   </si>
   <si>
@@ -234,9 +228,6 @@
     <t xml:space="preserve">Mechanical Mauraders</t>
   </si>
   <si>
-    <t xml:space="preserve">Robot Judge Grp 1</t>
-  </si>
-  <si>
     <t xml:space="preserve">108-i</t>
   </si>
   <si>
@@ -336,9 +327,6 @@
     <t xml:space="preserve">Explorers</t>
   </si>
   <si>
-    <t xml:space="preserve">Robot Judge Group 2</t>
-  </si>
-  <si>
     <t xml:space="preserve">202-ii</t>
   </si>
   <si>
@@ -378,9 +366,6 @@
     <t xml:space="preserve">Field 5 Grp 2</t>
   </si>
   <si>
-    <t xml:space="preserve">Field 5 Group 2</t>
-  </si>
-  <si>
     <t xml:space="preserve">124-i</t>
   </si>
   <si>
@@ -480,9 +465,6 @@
     <t xml:space="preserve">The Cheesy Poofs</t>
   </si>
   <si>
-    <t xml:space="preserve">Robot Judge Group 3</t>
-  </si>
-  <si>
     <t xml:space="preserve">219-i</t>
   </si>
   <si>
@@ -525,9 +507,6 @@
     <t xml:space="preserve">CyberSonics</t>
   </si>
   <si>
-    <t xml:space="preserve">Project Judge Grp3</t>
-  </si>
-  <si>
     <t xml:space="preserve">ModE-i</t>
   </si>
   <si>
@@ -582,9 +561,6 @@
     <t xml:space="preserve">Juggernauts</t>
   </si>
   <si>
-    <t xml:space="preserve">Robot Judge Grp4</t>
-  </si>
-  <si>
     <t xml:space="preserve">ModH-i</t>
   </si>
   <si>
@@ -622,9 +598,6 @@
   </si>
   <si>
     <t xml:space="preserve">NULL Team</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Project Judge 4</t>
   </si>
   <si>
     <t xml:space="preserve">ModJ-ii</t>
@@ -854,11 +827,11 @@
   <dimension ref="A1:AQ51"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B28" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
-      <selection pane="bottomRight" activeCell="B49" activeCellId="0" sqref="B49"/>
+      <selection pane="bottomLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
+      <selection pane="bottomRight" activeCell="H49" activeCellId="0" sqref="H49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1219,10 +1192,10 @@
         <v>43</v>
       </c>
       <c r="G4" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="I4" s="0" t="s">
         <v>43</v>
@@ -1234,7 +1207,7 @@
         <v>43</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="R4" s="3" t="s">
         <v>14</v>
@@ -1252,7 +1225,7 @@
         <v>24</v>
       </c>
       <c r="AC4" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AG4" s="7" t="s">
         <v>24</v>
@@ -1272,17 +1245,17 @@
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B5" s="6" t="n">
         <v>42069</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D5" s="2"/>
       <c r="F5" s="0" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="H5" s="0" t="s">
         <v>43</v>
@@ -1291,7 +1264,7 @@
         <v>44</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>43</v>
@@ -1315,7 +1288,7 @@
         <v>24</v>
       </c>
       <c r="AF5" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AG5" s="7" t="s">
         <v>24</v>
@@ -1335,20 +1308,20 @@
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B6" s="6" t="n">
         <v>24231</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D6" s="2"/>
       <c r="F6" s="0" t="s">
         <v>43</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="J6" s="0" t="s">
         <v>43</v>
@@ -1360,7 +1333,7 @@
         <v>43</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="R6" s="3" t="s">
         <v>14</v>
@@ -1378,7 +1351,7 @@
         <v>24</v>
       </c>
       <c r="AD6" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AG6" s="7" t="s">
         <v>24</v>
@@ -1398,62 +1371,62 @@
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B7" s="6" t="n">
         <v>14133</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="L7" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="K7" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="N7" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="R7" s="3" t="s">
         <v>14</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="W7" s="3" t="s">
         <v>19</v>
       </c>
       <c r="AA7" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="AB7" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AE7" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="AG7" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AI7" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="AL7" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AM7" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="AQ7" s="7" t="s">
         <v>24</v>
@@ -1461,62 +1434,62 @@
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B8" s="6" t="n">
         <v>13049</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="K8" s="3" t="s">
         <v>44</v>
       </c>
       <c r="L8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="P8" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="P8" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="R8" s="3" t="s">
         <v>14</v>
       </c>
       <c r="U8" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="W8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y8" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB8" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="AC8" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG8" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="AK8" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AL8" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="AO8" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="W8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y8" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="AB8" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="AC8" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="AG8" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="AK8" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="AL8" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="AO8" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="AQ8" s="7" t="s">
         <v>24</v>
@@ -1524,62 +1497,62 @@
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B9" s="6" t="n">
         <v>12954</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D9" s="2"/>
       <c r="F9" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="J9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="M9" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="K9" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="O9" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="R9" s="3" t="s">
         <v>14</v>
       </c>
       <c r="T9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="W9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="X9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB9" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="AF9" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="W9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="X9" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="AB9" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="AF9" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="AG9" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AJ9" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="AL9" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AN9" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="AQ9" s="7" t="s">
         <v>24</v>
@@ -1587,62 +1560,62 @@
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B10" s="6" t="n">
         <v>8978</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D10" s="2"/>
       <c r="F10" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="K10" s="3" t="s">
         <v>44</v>
       </c>
       <c r="M10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q10" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="Q10" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="R10" s="3" t="s">
         <v>14</v>
       </c>
       <c r="V10" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="W10" s="3" t="s">
         <v>19</v>
       </c>
       <c r="Z10" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="AB10" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AD10" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="AG10" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AH10" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="AL10" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AP10" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="AQ10" s="7" t="s">
         <v>24</v>
@@ -1650,62 +1623,62 @@
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B11" s="6" t="n">
         <v>7684</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="K11" s="3" t="s">
         <v>44</v>
       </c>
       <c r="N11" s="0" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="P11" s="0" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="R11" s="3" t="s">
         <v>14</v>
       </c>
       <c r="S11" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="W11" s="3" t="s">
         <v>19</v>
       </c>
       <c r="AA11" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="AB11" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AE11" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="AG11" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AI11" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="AL11" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AM11" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="AQ11" s="7" t="s">
         <v>24</v>
@@ -1713,62 +1686,62 @@
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B12" s="6" t="n">
         <v>6667</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D12" s="2"/>
       <c r="G12" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="K12" s="3" t="s">
         <v>44</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="R12" s="3" t="s">
         <v>14</v>
       </c>
       <c r="U12" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="W12" s="3" t="s">
         <v>19</v>
       </c>
       <c r="Y12" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="AB12" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AC12" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="AG12" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AK12" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="AL12" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AO12" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="AQ12" s="7" t="s">
         <v>24</v>
@@ -1776,62 +1749,62 @@
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B13" s="6" t="n">
         <v>5788</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D13" s="2"/>
       <c r="F13" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="K13" s="3" t="s">
         <v>44</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="R13" s="3" t="s">
         <v>14</v>
       </c>
       <c r="T13" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="W13" s="3" t="s">
         <v>19</v>
       </c>
       <c r="X13" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="AB13" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AF13" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="AG13" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AJ13" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="AL13" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AN13" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="AQ13" s="7" t="s">
         <v>24</v>
@@ -1839,62 +1812,62 @@
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B14" s="6" t="n">
         <v>5692</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D14" s="2"/>
       <c r="H14" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="K14" s="3" t="s">
         <v>44</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="R14" s="3" t="s">
         <v>14</v>
       </c>
       <c r="V14" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="W14" s="3" t="s">
         <v>19</v>
       </c>
       <c r="Z14" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="AB14" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AD14" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="AG14" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AH14" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="AL14" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AP14" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="AQ14" s="7" t="s">
         <v>24</v>
@@ -1902,62 +1875,62 @@
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B15" s="6" t="n">
         <v>5422</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="R15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="S15" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="K15" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="P15" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="R15" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="S15" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="W15" s="3" t="s">
         <v>19</v>
       </c>
       <c r="AA15" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="AB15" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AE15" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="AG15" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AI15" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="AL15" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AM15" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="AQ15" s="7" t="s">
         <v>24</v>
@@ -1965,62 +1938,62 @@
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B16" s="6" t="n">
         <v>5420</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G16" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="R16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="U16" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="I16" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="K16" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="N16" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="R16" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="U16" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="W16" s="3" t="s">
         <v>19</v>
       </c>
       <c r="Y16" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="AB16" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AC16" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="AG16" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AK16" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="AL16" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AO16" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="AQ16" s="7" t="s">
         <v>24</v>
@@ -2028,62 +2001,62 @@
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B17" s="6" t="n">
         <v>5181</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D17" s="2"/>
       <c r="F17" s="1" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="K17" s="3" t="s">
         <v>44</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="R17" s="3" t="s">
         <v>14</v>
       </c>
       <c r="T17" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="W17" s="3" t="s">
         <v>19</v>
       </c>
       <c r="X17" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="AB17" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AF17" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="AG17" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AJ17" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="AL17" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AN17" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="AQ17" s="7" t="s">
         <v>24</v>
@@ -2091,62 +2064,62 @@
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B18" s="6" t="n">
         <v>4750</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D18" s="2"/>
       <c r="F18" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="H18" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="R18" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="V18" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="J18" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="K18" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="M18" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="O18" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="R18" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="V18" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="W18" s="3" t="s">
         <v>19</v>
       </c>
       <c r="Z18" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="AB18" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AD18" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="AG18" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AH18" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="AL18" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AP18" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="AQ18" s="7" t="s">
         <v>24</v>
@@ -2154,62 +2127,62 @@
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B19" s="6" t="n">
         <v>4454</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D19" s="2"/>
       <c r="F19" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K19" s="3" t="s">
         <v>44</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="R19" s="3" t="s">
         <v>14</v>
       </c>
       <c r="T19" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="W19" s="3" t="s">
         <v>19</v>
       </c>
       <c r="X19" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="AB19" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AF19" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="AG19" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AJ19" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="AL19" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AN19" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="AQ19" s="7" t="s">
         <v>24</v>
@@ -2217,62 +2190,62 @@
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B20" s="6" t="n">
         <v>2607</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D20" s="2"/>
       <c r="F20" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="K20" s="3" t="s">
         <v>44</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="R20" s="3" t="s">
         <v>14</v>
       </c>
       <c r="V20" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="W20" s="3" t="s">
         <v>19</v>
       </c>
       <c r="Z20" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="AB20" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AD20" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="AG20" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AH20" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="AL20" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AP20" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="AQ20" s="7" t="s">
         <v>24</v>
@@ -2280,65 +2253,65 @@
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B21" s="6" t="n">
         <v>2590</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K21" s="3" t="s">
         <v>44</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="R21" s="3" t="s">
         <v>14</v>
       </c>
       <c r="S21" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="W21" s="3" t="s">
         <v>19</v>
       </c>
       <c r="AA21" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="AB21" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AE21" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="AG21" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AI21" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="AL21" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AM21" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="AQ21" s="7" t="s">
         <v>24</v>
@@ -2346,62 +2319,62 @@
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B22" s="6" t="n">
         <v>2539</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="K22" s="3" t="s">
         <v>44</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="R22" s="3" t="s">
         <v>14</v>
       </c>
       <c r="U22" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="W22" s="3" t="s">
         <v>19</v>
       </c>
       <c r="Y22" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="AB22" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AC22" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="AG22" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AK22" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="AL22" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AO22" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="AQ22" s="7" t="s">
         <v>24</v>
@@ -2409,62 +2382,62 @@
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B23" s="6" t="n">
         <v>2450</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="K23" s="3" t="s">
         <v>44</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="R23" s="3" t="s">
         <v>14</v>
       </c>
       <c r="S23" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="W23" s="3" t="s">
         <v>19</v>
       </c>
       <c r="AA23" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="AB23" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AE23" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="AG23" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AI23" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="AL23" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AM23" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="AQ23" s="7" t="s">
         <v>24</v>
@@ -2472,62 +2445,62 @@
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B24" s="6" t="n">
         <v>1218</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="D24" s="2"/>
       <c r="G24" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="K24" s="3" t="s">
         <v>44</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="R24" s="3" t="s">
         <v>14</v>
       </c>
       <c r="U24" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="W24" s="3" t="s">
         <v>19</v>
       </c>
       <c r="Y24" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="AB24" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AC24" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="AG24" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AK24" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="AL24" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AO24" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="AQ24" s="7" t="s">
         <v>24</v>
@@ -2535,62 +2508,62 @@
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="8" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B25" s="6" t="n">
         <v>709</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D25" s="2"/>
       <c r="F25" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="K25" s="3" t="s">
         <v>44</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="R25" s="3" t="s">
         <v>14</v>
       </c>
       <c r="T25" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="W25" s="3" t="s">
         <v>19</v>
       </c>
       <c r="X25" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="AB25" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AF25" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="AG25" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AJ25" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="AL25" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AN25" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="AQ25" s="7" t="s">
         <v>24</v>
@@ -2598,62 +2571,62 @@
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="8" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B26" s="6" t="n">
         <v>708</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D26" s="2"/>
       <c r="H26" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="K26" s="3" t="s">
         <v>44</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="Q26" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="R26" s="3" t="s">
         <v>14</v>
       </c>
       <c r="V26" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="W26" s="3" t="s">
         <v>19</v>
       </c>
       <c r="Z26" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="AB26" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AD26" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="AG26" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AH26" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="AL26" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AP26" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="AQ26" s="7" t="s">
         <v>24</v>
@@ -2661,62 +2634,62 @@
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B27" s="6" t="n">
         <v>607</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="K27" s="3" t="s">
         <v>44</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="R27" s="3" t="s">
         <v>14</v>
       </c>
       <c r="S27" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="W27" s="3" t="s">
         <v>19</v>
       </c>
       <c r="X27" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="AB27" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AC27" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="AG27" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AH27" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="AL27" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AM27" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="AQ27" s="7" t="s">
         <v>24</v>
@@ -2724,62 +2697,62 @@
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B28" s="6" t="n">
         <v>433</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="I28" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="G28" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>126</v>
-      </c>
       <c r="K28" s="3" t="s">
         <v>44</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="R28" s="3" t="s">
         <v>14</v>
       </c>
       <c r="U28" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="W28" s="3" t="s">
         <v>19</v>
       </c>
       <c r="Z28" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="AB28" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AE28" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="AG28" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AJ28" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="AL28" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AO28" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="AQ28" s="7" t="s">
         <v>24</v>
@@ -2787,62 +2760,62 @@
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B29" s="6" t="n">
         <v>365</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D29" s="2"/>
       <c r="F29" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="K29" s="3" t="s">
         <v>44</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="O29" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="Q29" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="R29" s="3" t="s">
         <v>14</v>
       </c>
       <c r="T29" s="1" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="W29" s="3" t="s">
         <v>19</v>
       </c>
       <c r="Y29" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="AB29" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AD29" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="AG29" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AI29" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="AL29" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AN29" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="AQ29" s="7" t="s">
         <v>24</v>
@@ -2850,62 +2823,62 @@
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B30" s="6" t="n">
         <v>321</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="D30" s="2"/>
       <c r="F30" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="K30" s="3" t="s">
         <v>44</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="O30" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="R30" s="3" t="s">
         <v>14</v>
       </c>
       <c r="V30" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="W30" s="3" t="s">
         <v>19</v>
       </c>
       <c r="AA30" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="AB30" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AF30" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="AG30" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AK30" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="AL30" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AP30" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="AQ30" s="7" t="s">
         <v>24</v>
@@ -2913,62 +2886,62 @@
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B31" s="6" t="n">
         <v>303</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="1" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="K31" s="3" t="s">
         <v>44</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="P31" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="R31" s="3" t="s">
         <v>14</v>
       </c>
       <c r="S31" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="W31" s="3" t="s">
         <v>19</v>
       </c>
       <c r="X31" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="AB31" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AC31" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="AG31" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AH31" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="AL31" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AM31" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="AQ31" s="7" t="s">
         <v>24</v>
@@ -2976,62 +2949,62 @@
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B32" s="6" t="n">
         <v>254</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="K32" s="3" t="s">
         <v>44</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>139</v>
+        <v>115</v>
       </c>
       <c r="P32" s="1" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="R32" s="3" t="s">
         <v>14</v>
       </c>
       <c r="U32" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="W32" s="3" t="s">
         <v>19</v>
       </c>
       <c r="Z32" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="AB32" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AE32" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="AG32" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AJ32" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="AL32" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AO32" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="AQ32" s="7" t="s">
         <v>24</v>
@@ -3039,62 +3012,62 @@
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B33" s="6" t="n">
         <v>225</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="D33" s="2"/>
       <c r="F33" s="1" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="K33" s="3" t="s">
         <v>44</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="O33" s="1" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="Q33" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="R33" s="3" t="s">
         <v>14</v>
       </c>
       <c r="T33" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="W33" s="3" t="s">
         <v>19</v>
       </c>
       <c r="Y33" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="AB33" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AD33" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="AG33" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AI33" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="AL33" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AN33" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="AQ33" s="7" t="s">
         <v>24</v>
@@ -3102,62 +3075,62 @@
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B34" s="6" t="n">
         <v>224</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="D34" s="2"/>
       <c r="F34" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="K34" s="3" t="s">
         <v>44</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="Q34" s="1" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="R34" s="3" t="s">
         <v>14</v>
       </c>
       <c r="V34" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="W34" s="3" t="s">
         <v>19</v>
       </c>
       <c r="AA34" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="AB34" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AF34" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="AG34" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AK34" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="AL34" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AP34" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="AQ34" s="7" t="s">
         <v>24</v>
@@ -3165,62 +3138,62 @@
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B35" s="6" t="n">
         <v>223</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="1" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="K35" s="3" t="s">
         <v>44</v>
       </c>
       <c r="N35" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="P35" s="1" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="R35" s="3" t="s">
         <v>14</v>
       </c>
       <c r="S35" s="1" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="W35" s="3" t="s">
         <v>19</v>
       </c>
       <c r="X35" s="1" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="AB35" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AC35" s="1" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="AG35" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AH35" s="1" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="AL35" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AM35" s="1" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="AQ35" s="7" t="s">
         <v>24</v>
@@ -3228,62 +3201,62 @@
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B36" s="6" t="n">
         <v>222</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="D36" s="2"/>
       <c r="G36" s="1" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="K36" s="3" t="s">
         <v>44</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="N36" s="1" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="P36" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="R36" s="3" t="s">
         <v>14</v>
       </c>
       <c r="U36" s="1" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="W36" s="3" t="s">
         <v>19</v>
       </c>
       <c r="Z36" s="1" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="AB36" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AE36" s="1" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="AG36" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AJ36" s="1" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="AL36" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AO36" s="1" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="AQ36" s="7" t="s">
         <v>24</v>
@@ -3291,62 +3264,62 @@
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B37" s="6" t="n">
         <v>193</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D37" s="2"/>
       <c r="F37" s="1" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="K37" s="3" t="s">
         <v>44</v>
       </c>
       <c r="O37" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="Q37" s="1" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="R37" s="3" t="s">
         <v>14</v>
       </c>
       <c r="T37" s="1" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="W37" s="3" t="s">
         <v>19</v>
       </c>
       <c r="Y37" s="1" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="AB37" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AD37" s="1" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="AG37" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AI37" s="1" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="AL37" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AN37" s="1" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="AQ37" s="7" t="s">
         <v>24</v>
@@ -3354,62 +3327,62 @@
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B38" s="6" t="n">
         <v>103</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="D38" s="2"/>
       <c r="H38" s="1" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>154</v>
+        <v>117</v>
       </c>
       <c r="K38" s="3" t="s">
         <v>44</v>
       </c>
       <c r="M38" s="1" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="O38" s="1" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="Q38" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="R38" s="3" t="s">
         <v>14</v>
       </c>
       <c r="V38" s="1" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="W38" s="3" t="s">
         <v>19</v>
       </c>
       <c r="AA38" s="1" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="AB38" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AF38" s="1" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="AG38" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AK38" s="1" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="AL38" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AP38" s="1" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="AQ38" s="7" t="s">
         <v>24</v>
@@ -3417,62 +3390,62 @@
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="B39" s="6" t="n">
         <v>102</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" s="1" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="K39" s="3" t="s">
         <v>44</v>
       </c>
       <c r="L39" s="1" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="N39" s="1" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="P39" s="1" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="R39" s="3" t="s">
         <v>14</v>
       </c>
       <c r="S39" s="1" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="W39" s="3" t="s">
         <v>19</v>
       </c>
       <c r="X39" s="1" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="AB39" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AC39" s="1" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="AG39" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AH39" s="1" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="AL39" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AM39" s="1" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="AQ39" s="7" t="s">
         <v>24</v>
@@ -3480,59 +3453,59 @@
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="B40" s="6" t="n">
         <v>75</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" s="1" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="K40" s="3" t="s">
         <v>44</v>
       </c>
       <c r="L40" s="1" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="N40" s="1" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="R40" s="3" t="s">
         <v>14</v>
       </c>
       <c r="U40" s="1" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="W40" s="3" t="s">
         <v>19</v>
       </c>
       <c r="Z40" s="1" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="AB40" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AE40" s="1" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="AG40" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AJ40" s="1" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="AL40" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AO40" s="1" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="AQ40" s="7" t="s">
         <v>24</v>
@@ -3540,62 +3513,62 @@
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="B41" s="6" t="n">
         <v>25</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="D41" s="2"/>
       <c r="F41" s="1" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="K41" s="3" t="s">
         <v>44</v>
       </c>
       <c r="M41" s="1" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="O41" s="1" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="Q41" s="1" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="R41" s="3" t="s">
         <v>14</v>
       </c>
       <c r="T41" s="1" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="W41" s="3" t="s">
         <v>19</v>
       </c>
       <c r="Y41" s="1" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="AB41" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AD41" s="1" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="AG41" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AI41" s="1" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="AL41" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AN41" s="1" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="AQ41" s="7" t="s">
         <v>24</v>
@@ -3603,62 +3576,62 @@
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="B42" s="6" t="n">
         <v>11</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="D42" s="2"/>
       <c r="F42" s="1" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="K42" s="3" t="s">
         <v>44</v>
       </c>
       <c r="M42" s="1" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="O42" s="1" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="R42" s="3" t="s">
         <v>14</v>
       </c>
       <c r="V42" s="1" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="W42" s="3" t="s">
         <v>19</v>
       </c>
       <c r="AA42" s="1" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="AB42" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AF42" s="1" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="AG42" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AK42" s="1" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="AL42" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AP42" s="1" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="AQ42" s="7" t="s">
         <v>24</v>
@@ -3666,59 +3639,59 @@
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="B43" s="6" t="n">
         <v>4</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" s="1" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="K43" s="3" t="s">
         <v>44</v>
       </c>
       <c r="L43" s="1" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="P43" s="1" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="R43" s="3" t="s">
         <v>14</v>
       </c>
       <c r="S43" s="1" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="W43" s="3" t="s">
         <v>19</v>
       </c>
       <c r="X43" s="1" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="AB43" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AC43" s="1" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="AG43" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AH43" s="1" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="AL43" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AM43" s="1" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="AQ43" s="7" t="s">
         <v>24</v>
@@ -3726,62 +3699,62 @@
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="B44" s="6" t="n">
         <v>1</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" s="1" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="I44" s="0" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="K44" s="3" t="s">
         <v>44</v>
       </c>
       <c r="L44" s="1" t="s">
-        <v>173</v>
+        <v>150</v>
       </c>
       <c r="P44" s="1" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="R44" s="3" t="s">
         <v>14</v>
       </c>
       <c r="U44" s="1" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="W44" s="3" t="s">
         <v>19</v>
       </c>
       <c r="Z44" s="1" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="AB44" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AE44" s="1" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="AG44" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AJ44" s="1" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="AL44" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AO44" s="1" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="AQ44" s="7" t="s">
         <v>24</v>
@@ -3789,62 +3762,62 @@
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="B45" s="0" t="n">
         <v>5555</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="D45" s="2"/>
       <c r="F45" s="1" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="K45" s="3" t="s">
         <v>44</v>
       </c>
       <c r="M45" s="1" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="O45" s="1" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="Q45" s="1" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="R45" s="3" t="s">
         <v>14</v>
       </c>
       <c r="T45" s="1" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="W45" s="3" t="s">
         <v>19</v>
       </c>
       <c r="Y45" s="1" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="AB45" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AD45" s="1" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="AG45" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AI45" s="1" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="AL45" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AN45" s="1" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="AQ45" s="7" t="s">
         <v>24</v>
@@ -3852,62 +3825,62 @@
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="B46" s="0" t="n">
         <v>666</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="D46" s="2"/>
       <c r="F46" s="1" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="K46" s="3" t="s">
         <v>44</v>
       </c>
       <c r="M46" s="1" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="Q46" s="1" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="R46" s="3" t="s">
         <v>14</v>
       </c>
       <c r="V46" s="1" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="W46" s="3" t="s">
         <v>19</v>
       </c>
       <c r="AA46" s="1" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="AB46" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AF46" s="1" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="AG46" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AK46" s="1" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="AL46" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AP46" s="1" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="AQ46" s="7" t="s">
         <v>24</v>
@@ -3915,62 +3888,62 @@
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="B47" s="0" t="n">
         <v>84686</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" s="1" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="K47" s="3" t="s">
         <v>44</v>
       </c>
       <c r="N47" s="1" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="P47" s="1" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="R47" s="3" t="s">
         <v>14</v>
       </c>
       <c r="S47" s="1" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="W47" s="3" t="s">
         <v>19</v>
       </c>
       <c r="X47" s="1" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="AB47" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AC47" s="1" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="AG47" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AH47" s="1" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="AL47" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AM47" s="1" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="AQ47" s="7" t="s">
         <v>24</v>
@@ -3978,62 +3951,62 @@
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="B48" s="0" t="n">
         <v>675613387</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="D48" s="2"/>
       <c r="G48" s="1" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="K48" s="3" t="s">
         <v>44</v>
       </c>
       <c r="L48" s="1" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="N48" s="1" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="P48" s="1" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="R48" s="3" t="s">
         <v>14</v>
       </c>
       <c r="U48" s="1" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="W48" s="3" t="s">
         <v>19</v>
       </c>
       <c r="Z48" s="1" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="AB48" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AE48" s="1" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="AG48" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AJ48" s="1" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="AL48" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AO48" s="1" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="AQ48" s="7" t="s">
         <v>24</v>
@@ -4041,62 +4014,62 @@
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="B49" s="0" t="n">
         <v>9999999</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="D49" s="2"/>
       <c r="F49" s="1" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>187</v>
+        <v>152</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="K49" s="3" t="s">
         <v>44</v>
       </c>
       <c r="O49" s="1" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="Q49" s="1" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="R49" s="3" t="s">
         <v>14</v>
       </c>
       <c r="T49" s="1" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="W49" s="3" t="s">
         <v>19</v>
       </c>
       <c r="Y49" s="1" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="AB49" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AD49" s="1" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="AG49" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AI49" s="1" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="AL49" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AN49" s="1" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="AQ49" s="7" t="s">
         <v>24</v>
@@ -4104,62 +4077,62 @@
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="B50" s="0" t="n">
         <v>2020</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="D50" s="2"/>
       <c r="H50" s="1" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="K50" s="3" t="s">
         <v>44</v>
       </c>
       <c r="M50" s="1" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="O50" s="1" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="Q50" s="1" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="R50" s="3" t="s">
         <v>14</v>
       </c>
       <c r="V50" s="1" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="W50" s="3" t="s">
         <v>19</v>
       </c>
       <c r="AA50" s="1" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="AB50" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AF50" s="1" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="AG50" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AK50" s="1" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="AL50" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AP50" s="1" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="AQ50" s="7" t="s">
         <v>24</v>
@@ -4167,7 +4140,7 @@
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C51" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished the current round of scheduling
</commit_message>
<xml_diff>
--- a/SRC/FLL Schedule.xlsx
+++ b/SRC/FLL Schedule.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jake/Documents/Robots/FLLTuneUpScheduleChecker/SRC/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Install\Desktop\Jake Code\FLLTuneUpScheduleChecker\SRC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{581C3893-46FC-DE4D-B9B3-56A065BB8908}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="12500" windowHeight="16060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="12495" windowHeight="16065" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,12 +30,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="A25" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="A25" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -79,7 +78,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A35" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="A35" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -625,13 +624,13 @@
     <t>4-H Robust Minds Robotics</t>
   </si>
   <si>
-    <t>No Entry</t>
+    <t>NO TEAM SKIP THIS SLOT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="hh:mm:ss\ AM/PM"/>
   </numFmts>
@@ -873,6 +872,102 @@
             <a:srgbClr val="000000"/>
           </a:solidFill>
           <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="AutoShape 4"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12696825" cy="12696825"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12696825" cy="12696825"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
           <a:headEnd/>
           <a:tailEnd/>
         </a:ln>
@@ -1179,42 +1274,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AQ51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A28" sqref="A28"/>
-      <selection pane="bottomRight" activeCell="C17" sqref="C17"/>
+      <selection pane="bottomRight" activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="9.5" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" customWidth="1"/>
-    <col min="3" max="3" width="35.33203125" customWidth="1"/>
-    <col min="4" max="4" width="7.33203125" customWidth="1"/>
-    <col min="5" max="6" width="19.83203125" customWidth="1"/>
-    <col min="7" max="7" width="20.5" customWidth="1"/>
-    <col min="8" max="8" width="19.6640625" customWidth="1"/>
-    <col min="9" max="10" width="17.33203125" customWidth="1"/>
-    <col min="11" max="11" width="15.1640625" customWidth="1"/>
-    <col min="12" max="12" width="19.33203125" customWidth="1"/>
-    <col min="13" max="17" width="17.33203125" customWidth="1"/>
-    <col min="18" max="18" width="16.5" customWidth="1"/>
-    <col min="19" max="22" width="17.6640625" customWidth="1"/>
-    <col min="23" max="23" width="21.1640625" customWidth="1"/>
-    <col min="24" max="27" width="17.6640625" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+    <col min="3" max="3" width="35.28515625" customWidth="1"/>
+    <col min="4" max="4" width="7.28515625" customWidth="1"/>
+    <col min="5" max="6" width="19.85546875" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" customWidth="1"/>
+    <col min="8" max="8" width="19.7109375" customWidth="1"/>
+    <col min="9" max="10" width="17.28515625" customWidth="1"/>
+    <col min="11" max="11" width="15.140625" customWidth="1"/>
+    <col min="12" max="12" width="19.28515625" customWidth="1"/>
+    <col min="13" max="17" width="17.28515625" customWidth="1"/>
+    <col min="18" max="18" width="16.42578125" customWidth="1"/>
+    <col min="19" max="22" width="17.7109375" customWidth="1"/>
+    <col min="23" max="23" width="21.140625" customWidth="1"/>
+    <col min="24" max="27" width="17.7109375" customWidth="1"/>
     <col min="28" max="28" width="15" customWidth="1"/>
-    <col min="29" max="30" width="13.6640625" customWidth="1"/>
-    <col min="31" max="32" width="17.6640625" customWidth="1"/>
+    <col min="29" max="30" width="13.7109375" customWidth="1"/>
+    <col min="31" max="32" width="17.7109375" customWidth="1"/>
     <col min="33" max="33" width="15" customWidth="1"/>
-    <col min="34" max="37" width="17.6640625" customWidth="1"/>
+    <col min="34" max="37" width="17.7109375" customWidth="1"/>
     <col min="38" max="38" width="15" customWidth="1"/>
-    <col min="39" max="42" width="17.6640625" customWidth="1"/>
-    <col min="43" max="43" width="13.6640625" customWidth="1"/>
-    <col min="44" max="1025" width="14.5" customWidth="1"/>
+    <col min="39" max="42" width="17.7109375" customWidth="1"/>
+    <col min="43" max="43" width="13.7109375" customWidth="1"/>
+    <col min="44" max="1025" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="12.75" customHeight="1">

</xml_diff>